<commit_message>
this is my twentythird commit
</commit_message>
<xml_diff>
--- a/testData/TC_CreateDirectOpportunity.xlsx
+++ b/testData/TC_CreateDirectOpportunity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilr2\eclipse-workspace\UCPQ_Automation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E307D19-5DEF-4422-8D0F-98F8A8343996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ACA160-32CC-43ED-B02E-D5BE71432996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,11 +205,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -503,7 +503,7 @@
     <col min="1" max="1" width="26.07421875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.3828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.3046875" customWidth="1"/>
-    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.3828125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.07421875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
@@ -515,46 +515,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
this is my twentyfourth commit
</commit_message>
<xml_diff>
--- a/testData/TC_CreateDirectOpportunity.xlsx
+++ b/testData/TC_CreateDirectOpportunity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunilr2\eclipse-workspace\UCPQ_Automation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ACA160-32CC-43ED-B02E-D5BE71432996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8934D2-2BE1-4C90-A68E-F49F09E06F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Direct</t>
+  </si>
+  <si>
+    <t>Hyperscaler</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection sqref="A1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -509,12 +512,13 @@
     <col min="7" max="7" width="15.07421875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.61328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.3828125" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="17.3828125" customWidth="1"/>
+    <col min="11" max="11" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.3828125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.3828125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="17.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -533,8 +537,9 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -555,8 +560,9 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,25 +594,28 @@
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -643,11 +652,12 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{147F5B5B-A653-4F7A-9371-88FE8BC0D8D7}"/>

</xml_diff>